<commit_message>
Arranging Getting Organized modules
</commit_message>
<xml_diff>
--- a/resources/Dates_207.xlsx
+++ b/resources/Dates_207.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="90">
   <si>
     <t>url</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>Case Studies</t>
+  </si>
+  <si>
+    <t>Getting Organized I</t>
+  </si>
+  <si>
+    <t>GetOrganized1</t>
+  </si>
+  <si>
+    <t>GetOrganized2</t>
   </si>
 </sst>
 </file>
@@ -670,7 +679,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,10 +716,10 @@
         <v>44573</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,7 +737,7 @@
         <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>